<commit_message>
update and delete commit
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bf84e1838b3daa6/Documents/UiPath/CMPG-323-Project-4-31846769/Connected Office Web Application User Acceptance Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{5546F926-6C85-4EAE-890A-D0833008B810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5069F911-C3F2-481E-9155-C731F0F82983}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{5546F926-6C85-4EAE-890A-D0833008B810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC6D3FC1-7924-4D50-80AE-06FE5F03958D}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,6 +431,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>